<commit_message>
Simon this is for yougit add .
</commit_message>
<xml_diff>
--- a/Exercice1.45.xlsx
+++ b/Exercice1.45.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Desktop\CompSci\projects\ECSE 420\ecse420f2018-PS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mystelvric/Documents/Mcgill/Fall 2018/ECSE 420/Assignments/ecse420f2018-PS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DACE658C-1244-41CF-8AAC-F28908F9F2E0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C797BB47-F47A-AD47-B368-3877EA0BFFDD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12800" windowHeight="4730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exec times" sheetId="3" r:id="rId1"/>
@@ -103,7 +103,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -135,7 +135,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Execution time per number of threads on 2000x2000 matrices</a:t>
+              <a:t>Parallel Execution time per number of threads on 2000x2000 matrices</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -170,16 +170,16 @@
               <a:cs typeface="+mj-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="1"/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -194,43 +194,34 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="6"/>
-          </c:marker>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="6"/>
-              <c:spPr>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
                 <a:solidFill>
-                  <a:schemeClr val="lt1"/>
+                  <a:schemeClr val="accent1"/>
                 </a:solidFill>
-                <a:ln w="38100">
-                  <a:solidFill>
-                    <a:schemeClr val="accent1">
-                      <a:shade val="42000"/>
-                      <a:alpha val="60000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:shade val="42000"/>
-                    <a:alpha val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
+                <a:prstDash val="solid"/>
                 <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-238F-418B-8893-67755C19945B}"/>
@@ -239,37 +230,7 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="6"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:ln w="38100">
-                  <a:solidFill>
-                    <a:schemeClr val="accent1">
-                      <a:shade val="55000"/>
-                      <a:alpha val="60000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:shade val="55000"/>
-                    <a:alpha val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-238F-418B-8893-67755C19945B}"/>
@@ -278,37 +239,7 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="6"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:ln w="38100">
-                  <a:solidFill>
-                    <a:schemeClr val="accent1">
-                      <a:shade val="68000"/>
-                      <a:alpha val="60000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:shade val="68000"/>
-                    <a:alpha val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-238F-418B-8893-67755C19945B}"/>
@@ -317,37 +248,7 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="6"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:ln w="38100">
-                  <a:solidFill>
-                    <a:schemeClr val="accent1">
-                      <a:shade val="80000"/>
-                      <a:alpha val="60000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:shade val="80000"/>
-                    <a:alpha val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000007-238F-418B-8893-67755C19945B}"/>
@@ -356,37 +257,7 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="6"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:ln w="38100">
-                  <a:solidFill>
-                    <a:schemeClr val="accent1">
-                      <a:shade val="93000"/>
-                      <a:alpha val="60000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:shade val="93000"/>
-                    <a:alpha val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000009-238F-418B-8893-67755C19945B}"/>
@@ -395,37 +266,7 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="6"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:ln w="38100">
-                  <a:solidFill>
-                    <a:schemeClr val="accent1">
-                      <a:tint val="94000"/>
-                      <a:alpha val="60000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:tint val="94000"/>
-                    <a:alpha val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000B-238F-418B-8893-67755C19945B}"/>
@@ -434,37 +275,7 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="6"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:ln w="38100">
-                  <a:solidFill>
-                    <a:schemeClr val="accent1">
-                      <a:tint val="81000"/>
-                      <a:alpha val="60000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:tint val="81000"/>
-                    <a:alpha val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000D-238F-418B-8893-67755C19945B}"/>
@@ -473,37 +284,7 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="6"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:ln w="38100">
-                  <a:solidFill>
-                    <a:schemeClr val="accent1">
-                      <a:tint val="69000"/>
-                      <a:alpha val="60000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:tint val="69000"/>
-                    <a:alpha val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000F-238F-418B-8893-67755C19945B}"/>
@@ -512,37 +293,7 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="6"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:ln w="38100">
-                  <a:solidFill>
-                    <a:schemeClr val="accent1">
-                      <a:tint val="56000"/>
-                      <a:alpha val="60000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:tint val="56000"/>
-                    <a:alpha val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000011-238F-418B-8893-67755C19945B}"/>
@@ -551,44 +302,82 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="6"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:ln w="38100">
-                  <a:solidFill>
-                    <a:schemeClr val="accent1">
-                      <a:tint val="43000"/>
-                      <a:alpha val="60000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:tint val="43000"/>
-                    <a:alpha val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000013-238F-418B-8893-67755C19945B}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
-          <c:xVal>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>, </c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000F-238F-418B-8893-67755C19945B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1"/>
+                      </a:solidFill>
+                      <a:prstDash val="solid"/>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
             <c:numRef>
               <c:f>'Exec times'!$B$3:$B$12</c:f>
               <c:numCache>
@@ -626,8 +415,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
+          </c:cat>
+          <c:val>
             <c:numRef>
               <c:f>'Exec times'!$C$3:$C$12</c:f>
               <c:numCache>
@@ -655,7 +444,7 @@
                   <c:v>7103</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6628</c:v>
+                  <c:v>6440</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>7029</c:v>
@@ -665,8 +454,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
+          </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000014-238F-418B-8893-67755C19945B}"/>
@@ -681,10 +470,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="448325504"/>
         <c:axId val="448325920"/>
-      </c:scatterChart>
-      <c:valAx>
+      </c:lineChart>
+      <c:catAx>
         <c:axId val="448325504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -700,12 +491,43 @@
                   <a:lumOff val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:prstDash val="solid"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>NUMBER</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR" baseline="0"/>
+                  <a:t> OF THREADS</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -731,7 +553,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="fr-FR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -741,13 +563,15 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
                 <a:lumMod val="25000"/>
                 <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -768,13 +592,16 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="448325920"/>
         <c:crosses val="min"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="448325920"/>
         <c:scaling>
@@ -791,12 +618,43 @@
                   <a:lumOff val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:prstDash val="solid"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>TIME</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR" baseline="0"/>
+                  <a:t> IN ms</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -822,7 +680,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="fr-FR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -832,13 +690,15 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
                 <a:lumMod val="25000"/>
                 <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -859,12 +719,12 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="448325504"/>
         <c:crosses val="min"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -889,6 +749,7 @@
           <a:lumOff val="85000"/>
         </a:schemeClr>
       </a:solidFill>
+      <a:prstDash val="solid"/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -900,7 +761,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -914,7 +775,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -975,7 +836,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -991,7 +852,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Exec times'!$F$2</c:f>
+              <c:f>'Exec times'!$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1062,7 +923,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Exec times'!$F$3:$F$8</c:f>
+              <c:f>'Exec times'!$H$3:$H$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1113,7 +974,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Exec times'!$G$2</c:f>
+              <c:f>'Exec times'!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1199,7 +1060,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Exec times'!$G$3:$G$8</c:f>
+              <c:f>'Exec times'!$F$3:$F$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1236,7 +1097,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Exec times'!$H$2</c:f>
+              <c:f>'Exec times'!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1322,7 +1183,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Exec times'!$H$3:$H$8</c:f>
+              <c:f>'Exec times'!$G$3:$G$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1333,7 +1194,7 @@
                   <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>157</c:v>
+                  <c:v>152</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>581</c:v>
@@ -1368,6 +1229,7 @@
       <c:valAx>
         <c:axId val="807815055"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1431,7 +1293,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="fr-FR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1460,7 +1322,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="807820047"/>
@@ -1538,7 +1400,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="fr-FR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1567,7 +1429,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="807815055"/>
@@ -1626,7 +1488,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="fr-FR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1655,10 +1517,11 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="578303919"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
@@ -1726,7 +1589,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="fr-FR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1761,10 +1624,11 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="807805487"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1802,7 +1666,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1839,7 +1703,566 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Execution time of squential</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" baseline="0"/>
+              <a:t> and parallel algorithm for different matri </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>(8 cores)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.9124890638670184E-2"/>
+          <c:y val="0.15780110819480897"/>
+          <c:w val="0.87754177602799655"/>
+          <c:h val="0.72094889180519106"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Sequential</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Exec times'!$E$3:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Exec times'!$F$3:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>367</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2110</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>46118</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1050512</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2964-8D48-88F8-68EEDD27620F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Parallel</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Exec times'!$E$3:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Exec times'!$G$3:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>581</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6628</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>172585</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-2964-8D48-88F8-68EEDD27620F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1998188335"/>
+        <c:axId val="1998864575"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1998188335"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Matrix Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1998864575"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1998864575"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR" baseline="0"/>
+                  <a:t> in ms log10</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1998188335"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1851,7 +2274,7 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="14">
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinearReversed" id="21">
   <a:schemeClr val="accent1"/>
 </cs:colorStyle>
 </file>
@@ -1893,43 +2316,105 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="249">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="103">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" cap="all"/>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
+    <cs:lnRef idx="1">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:tint val="75000"/>
       </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200" cap="none" spc="20" normalizeH="0" baseline="0"/>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1">
+        <a:tint val="75000"/>
+      </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <a:schemeClr val="bg1"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -1940,310 +2425,233 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln>
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="bg1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="50000"/>
-          <a:lumOff val="50000"/>
-        </a:schemeClr>
-      </a:solidFill>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:alpha val="70000"/>
-        </a:schemeClr>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:alpha val="70000"/>
-        </a:schemeClr>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="60000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="38100">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="60000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
     </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:lineWidthScale>3</cs:lineWidthScale>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln cap="rnd">
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1">
+        <a:tint val="75000"/>
+      </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1" mods="ignoreCSTransforms">
+      <cs:styleClr val="0">
+        <a:shade val="25000"/>
+      </cs:styleClr>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
   </cs:downBar>
   <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
         <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
   <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
         <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:errorBar>
   <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1">
+        <a:tint val="75000"/>
+      </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1">
+        <a:tint val="75000"/>
+      </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
         <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMajor>
   <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1">
+        <a:tint val="50000"/>
+      </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
   <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
         <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
   <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -2252,66 +2660,57 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" baseline="0"/>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:legend>
   <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1">
+      <a:schemeClr val="bg1"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
+    <cs:lnRef idx="1">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:tint val="75000"/>
       </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
         <a:round/>
       </a:ln>
     </cs:spPr>
@@ -2320,28 +2719,23 @@
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
-    <cs:fontRef idx="major">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1600" b="0" i="0" kern="1200" cap="none" spc="50" normalizeH="0" baseline="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200"/>
   </cs:title>
   <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
     </cs:lnRef>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="15875" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln cap="rnd">
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -2350,62 +2744,53 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:trendlineLabel>
   <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1" mods="ignoreCSTransforms">
+      <cs:styleClr val="0">
+        <a:tint val="25000"/>
+      </cs:styleClr>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
   <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
+    <cs:lnRef idx="1">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:tint val="75000"/>
       </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200" spc="20" baseline="0"/>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
@@ -2878,20 +3263,493 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>6350</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2920,16 +3778,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>85724</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>41274</xdr:rowOff>
+      <xdr:rowOff>66674</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2954,11 +3812,47 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>565150</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Graphique 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45657C19-BD39-B947-B965-537827E36F36}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3259,30 +4153,30 @@
   </sheetPr>
   <dimension ref="B1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="F21" workbookViewId="0">
+      <selection activeCell="P61" sqref="P61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" customWidth="1"/>
-    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" customWidth="1"/>
-    <col min="5" max="5" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.81640625" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15.5">
+    <row r="1" spans="2:8" ht="16">
       <c r="D1" s="1"/>
-      <c r="G1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="2:8" ht="15.5">
+    <row r="2" spans="2:8" ht="16">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -3294,16 +4188,16 @@
         <v>5</v>
       </c>
       <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="3" spans="2:8" ht="15.5">
+    <row r="3" spans="2:8" ht="16">
       <c r="B3">
         <v>1</v>
       </c>
@@ -3315,16 +4209,16 @@
         <v>100</v>
       </c>
       <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>31</v>
+      </c>
+      <c r="H3">
         <v>2</v>
       </c>
-      <c r="G3">
-        <v>10</v>
-      </c>
-      <c r="H3">
-        <v>31</v>
-      </c>
     </row>
-    <row r="4" spans="2:8" ht="15.5">
+    <row r="4" spans="2:8" ht="16">
       <c r="B4">
         <v>2</v>
       </c>
@@ -3336,16 +4230,16 @@
         <v>200</v>
       </c>
       <c r="F4">
+        <v>29</v>
+      </c>
+      <c r="G4">
+        <v>45</v>
+      </c>
+      <c r="H4">
         <v>2</v>
       </c>
-      <c r="G4">
-        <v>29</v>
-      </c>
-      <c r="H4">
-        <v>45</v>
-      </c>
     </row>
-    <row r="5" spans="2:8" ht="15.5">
+    <row r="5" spans="2:8" ht="16">
       <c r="B5">
         <v>3</v>
       </c>
@@ -3357,16 +4251,16 @@
         <v>500</v>
       </c>
       <c r="F5">
+        <v>367</v>
+      </c>
+      <c r="G5">
+        <v>152</v>
+      </c>
+      <c r="H5">
         <v>8</v>
       </c>
-      <c r="G5">
-        <v>367</v>
-      </c>
-      <c r="H5">
-        <v>157</v>
-      </c>
     </row>
-    <row r="6" spans="2:8" ht="15.5">
+    <row r="6" spans="2:8" ht="16">
       <c r="B6">
         <v>4</v>
       </c>
@@ -3378,16 +4272,16 @@
         <v>1000</v>
       </c>
       <c r="F6">
+        <v>2110</v>
+      </c>
+      <c r="G6">
+        <v>581</v>
+      </c>
+      <c r="H6">
         <v>8</v>
       </c>
-      <c r="G6">
-        <v>2110</v>
-      </c>
-      <c r="H6">
-        <v>581</v>
-      </c>
     </row>
-    <row r="7" spans="2:8" ht="15.5">
+    <row r="7" spans="2:8" ht="16">
       <c r="B7">
         <v>5</v>
       </c>
@@ -3399,16 +4293,16 @@
         <v>2000</v>
       </c>
       <c r="F7">
+        <v>46118</v>
+      </c>
+      <c r="G7">
+        <v>6628</v>
+      </c>
+      <c r="H7">
         <v>8</v>
       </c>
-      <c r="G7">
-        <v>46118</v>
-      </c>
-      <c r="H7">
-        <v>6628</v>
-      </c>
     </row>
-    <row r="8" spans="2:8" ht="15.5">
+    <row r="8" spans="2:8" ht="16">
       <c r="B8">
         <v>6</v>
       </c>
@@ -3420,16 +4314,16 @@
         <v>4000</v>
       </c>
       <c r="F8">
+        <v>1050512</v>
+      </c>
+      <c r="G8">
+        <v>172585</v>
+      </c>
+      <c r="H8">
         <v>8</v>
       </c>
-      <c r="G8">
-        <v>1050512</v>
-      </c>
-      <c r="H8">
-        <v>172585</v>
-      </c>
     </row>
-    <row r="9" spans="2:8" ht="15.5">
+    <row r="9" spans="2:8" ht="16">
       <c r="B9">
         <v>7</v>
       </c>
@@ -3442,12 +4336,12 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="2:8" ht="15.5">
+    <row r="10" spans="2:8" ht="16">
       <c r="B10">
         <v>8</v>
       </c>
       <c r="C10">
-        <v>6628</v>
+        <v>6440</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -3455,7 +4349,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="2:8" ht="15.5">
+    <row r="11" spans="2:8" ht="16">
       <c r="B11">
         <v>9</v>
       </c>
@@ -3468,7 +4362,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="2:8" ht="15.5">
+    <row r="12" spans="2:8" ht="16">
       <c r="B12">
         <v>10</v>
       </c>
@@ -3482,9 +4376,6 @@
       <c r="H12" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="G1:H1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>